<commit_message>
More figure adjustments and corresponding comment adjustments.
</commit_message>
<xml_diff>
--- a/2013/report-JAR/runnerup.xlsx
+++ b/2013/report-JAR/runnerup.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcok\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19350" windowHeight="9285" activeTab="1"/>
   </bookViews>
@@ -1740,11 +1735,11 @@
             <a:effectLst/>
           </c:spPr>
         </c:hiLowLines>
-        <c:axId val="212748912"/>
-        <c:axId val="212961616"/>
+        <c:axId val="46107648"/>
+        <c:axId val="46109440"/>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="212748912"/>
+        <c:axId val="46107648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1784,7 +1779,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="212961616"/>
+        <c:crossAx val="46109440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1792,7 +1787,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="212961616"/>
+        <c:axId val="46109440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1841,7 +1836,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="212748912"/>
+        <c:crossAx val="46107648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2450,16 +2445,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>419101</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2738,7 +2733,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3971,7 +3966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R44" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>